<commit_message>
Added the files to my branch
</commit_message>
<xml_diff>
--- a/Helix_UI_Framework/src/test/resources/TestData/Helix_Proj_Admin_Test_Data.xlsx
+++ b/Helix_UI_Framework/src/test/resources/TestData/Helix_Proj_Admin_Test_Data.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Helix_UI_POC\Helix_UI_Framework\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01614D84-F67F-431A-972A-27AFEE473FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Project_Admin_Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,15 +24,60 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Job code</t>
+  </si>
+  <si>
+    <t>SOW Fee</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Speaker Bureau1</t>
+  </si>
+  <si>
+    <t>Speaker Bureau2</t>
+  </si>
+  <si>
+    <t>Account Service1</t>
+  </si>
+  <si>
+    <t>Account Service2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +382,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+      <c r="C2">
+        <v>65</v>
+      </c>
+      <c r="D2">
+        <v>65</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the code for Helix project admin
</commit_message>
<xml_diff>
--- a/Helix_UI_Framework/src/test/resources/TestData/Helix_Proj_Admin_Test_Data.xlsx
+++ b/Helix_UI_Framework/src/test/resources/TestData/Helix_Proj_Admin_Test_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Helix_UI_POC\Helix_UI_Framework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01614D84-F67F-431A-972A-27AFEE473FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4E2158-3FC2-46A6-923D-7B737F8D05CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Job code</t>
   </si>
@@ -58,6 +58,117 @@
   </si>
   <si>
     <t>Account Service2</t>
+  </si>
+  <si>
+    <t>Chase_Card_limit</t>
+  </si>
+  <si>
+    <t>Honoraria_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Honoraria_Avg_unit</t>
+  </si>
+  <si>
+    <t>Airfare_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Airfare_Avg_unit</t>
+  </si>
+  <si>
+    <t>Speaker Ground Transportation_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Speaker Ground Transportation_Avg_unit</t>
+  </si>
+  <si>
+    <t>Speaker T&amp;E_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Speaker T&amp;E_Avg_unit</t>
+  </si>
+  <si>
+    <t>Speaker Lodging_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Speaker Lodging_Avg_unit</t>
+  </si>
+  <si>
+    <t>Venue Food and Beverage_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Venue Food and Beverage_Avg_unit</t>
+  </si>
+  <si>
+    <t>Management Fee_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Management Fee_Avg_unit</t>
+  </si>
+  <si>
+    <t>Late Fee_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Late Fee_Avg_unit</t>
+  </si>
+  <si>
+    <t>Cancellation Fee_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Cancellation Fee_Avg_unit</t>
+  </si>
+  <si>
+    <t>Onsite Planner_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Onsite Planner_Avg_unit</t>
+  </si>
+  <si>
+    <t>Audio Visual_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Audio Visual_Avg_unit</t>
+  </si>
+  <si>
+    <t>Virtual Host_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Virtual Host_Avg_unit</t>
+  </si>
+  <si>
+    <t>Catering Fee_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Catering Fee_Avg_unit</t>
+  </si>
+  <si>
+    <t>Virtual Catering Fee_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Virtual Catering Fee_Avg_unit</t>
+  </si>
+  <si>
+    <t>Honoraria Fee_Avg_unit</t>
+  </si>
+  <si>
+    <t>Honoraria Fee_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Mileage_Avg_unit</t>
+  </si>
+  <si>
+    <t>Mileage_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Circuit_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Circuit_Avg_unit</t>
+  </si>
+  <si>
+    <t>Travel Honoraria_Avg_quantity</t>
+  </si>
+  <si>
+    <t>Travel Honoraria_Avg_unit</t>
   </si>
 </sst>
 </file>
@@ -100,9 +211,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,86 +499,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AN4" sqref="AN4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:47" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>123</v>
       </c>
-      <c r="C2">
-        <v>65</v>
-      </c>
-      <c r="D2">
-        <v>65</v>
-      </c>
-      <c r="E2">
-        <v>12</v>
-      </c>
-      <c r="F2">
+      <c r="C2" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>4</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>3</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>6</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>100</v>
+      </c>
+      <c r="N2" s="1">
+        <v>2</v>
+      </c>
+      <c r="O2" s="1">
+        <v>100</v>
+      </c>
+      <c r="P2" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>200</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
+        <v>100</v>
+      </c>
+      <c r="T2" s="1">
+        <v>2</v>
+      </c>
+      <c r="U2" s="1">
+        <v>100</v>
+      </c>
+      <c r="V2" s="1">
+        <v>3</v>
+      </c>
+      <c r="W2" s="1">
+        <v>200</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>100</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>100</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>100</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>100</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>200</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>100</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>100</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>200</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>100</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>100</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the code for proj admin
</commit_message>
<xml_diff>
--- a/Helix_UI_Framework/src/test/resources/TestData/Helix_Proj_Admin_Test_Data.xlsx
+++ b/Helix_UI_Framework/src/test/resources/TestData/Helix_Proj_Admin_Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Helix_UI_POC\Helix_UI_Framework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4E2158-3FC2-46A6-923D-7B737F8D05CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987654AC-250F-4261-972A-E07CEB5D2A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Job code</t>
   </si>
@@ -169,6 +169,93 @@
   </si>
   <si>
     <t>Travel Honoraria_Avg_unit</t>
+  </si>
+  <si>
+    <t>LSF_LessThan</t>
+  </si>
+  <si>
+    <t>LSF_GThan</t>
+  </si>
+  <si>
+    <t>LSF_Per</t>
+  </si>
+  <si>
+    <t>LSF_Dollar</t>
+  </si>
+  <si>
+    <t>CFT_LessThan</t>
+  </si>
+  <si>
+    <t>CFT_GThan</t>
+  </si>
+  <si>
+    <t>CFT_Per</t>
+  </si>
+  <si>
+    <t>CFT_Dollar</t>
+  </si>
+  <si>
+    <t>VH_Per</t>
+  </si>
+  <si>
+    <t>VH_Dol</t>
+  </si>
+  <si>
+    <t>CF_Per</t>
+  </si>
+  <si>
+    <t>CF_Dol</t>
+  </si>
+  <si>
+    <t>VCF_Per</t>
+  </si>
+  <si>
+    <t>VCF_Dol</t>
+  </si>
+  <si>
+    <t>Other_fee_fld1</t>
+  </si>
+  <si>
+    <t>Other_fee_fld2</t>
+  </si>
+  <si>
+    <t>Other_fee_fld3</t>
+  </si>
+  <si>
+    <t>SCH_LessThan</t>
+  </si>
+  <si>
+    <t>SCH_GThan</t>
+  </si>
+  <si>
+    <t>SCH_Per</t>
+  </si>
+  <si>
+    <t>SCH_Dollar</t>
+  </si>
+  <si>
+    <t>Mileage_term_fld1</t>
+  </si>
+  <si>
+    <t>Mileage_term_fld2</t>
+  </si>
+  <si>
+    <t>Mileage_term_fld3</t>
+  </si>
+  <si>
+    <t>Circuit_fld1</t>
+  </si>
+  <si>
+    <t>THT_LessThan</t>
+  </si>
+  <si>
+    <t>THT_GThan</t>
+  </si>
+  <si>
+    <t>THT_Per</t>
+  </si>
+  <si>
+    <t>THT_Dollar</t>
   </si>
 </sst>
 </file>
@@ -499,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU2"/>
+  <dimension ref="A1:BX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AN4" sqref="AN4"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BP5" sqref="BP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +609,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:76" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,8 +751,95 @@
       <c r="AU1" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="AV1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -806,6 +980,93 @@
       </c>
       <c r="AU2" s="1">
         <v>200</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BB2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BN2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BO2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BP2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BR2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BT2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BU2" s="1">
+        <v>2</v>
+      </c>
+      <c r="BV2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the code for project admin flow
</commit_message>
<xml_diff>
--- a/Helix_UI_Framework/src/test/resources/TestData/Helix_Proj_Admin_Test_Data.xlsx
+++ b/Helix_UI_Framework/src/test/resources/TestData/Helix_Proj_Admin_Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Helix_UI_POC\Helix_UI_Framework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987654AC-250F-4261-972A-E07CEB5D2A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A381C4-CD52-4E91-B4CC-DB4C4C187280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t>Job code</t>
   </si>
@@ -586,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BX2"/>
+  <dimension ref="A1:CB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
-      <selection activeCell="BP5" sqref="BP5"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="BW2" sqref="BW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +609,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:80" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -838,8 +838,20 @@
       <c r="BX1" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="BY1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1057,7 +1069,7 @@
         <v>1</v>
       </c>
       <c r="BU2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BV2" s="1">
         <v>1</v>
@@ -1066,6 +1078,18 @@
         <v>1</v>
       </c>
       <c r="BX2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BY2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BZ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB2" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>